<commit_message>
GREEN in BUURT, METRICS
</commit_message>
<xml_diff>
--- a/R/neighbourhoods.xlsx
+++ b/R/neighbourhoods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RSTAT\REMOTESENSING\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94934271-A7AA-4B6B-BA45-44AD9F8E96A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3074A8FF-B58D-461A-94C2-36920CEB13C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="3240" windowWidth="25670" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15500" yWindow="1820" windowWidth="21990" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>BU08280002</t>
-  </si>
-  <si>
     <t>buurtcode</t>
   </si>
   <si>
     <t>gemeente</t>
+  </si>
+  <si>
+    <t>BU08280002</t>
   </si>
   <si>
     <t>Oss</t>
@@ -400,7 +400,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -410,15 +410,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
TREE CROWNS & -TOPS
</commit_message>
<xml_diff>
--- a/R/neighbourhoods.xlsx
+++ b/R/neighbourhoods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RSTAT\REMOTESENSING\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3D828BDB-3EE4-40EC-B309-6CF59745A9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3CA5D310-B7AD-44E9-9BBA-A83D2368BFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,23 +46,30 @@
     <t>gemeente</t>
   </si>
   <si>
-    <t>BU08280002</t>
+    <t>BU15810004</t>
   </si>
   <si>
-    <t>Oss</t>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,7 +412,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,7 +426,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -427,5 +435,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CHM SMOOTHING, TREE TOP DETECTION, CANOPY
</commit_message>
<xml_diff>
--- a/R/neighbourhoods.xlsx
+++ b/R/neighbourhoods.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RSTAT\REMOTESENSING\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATASCIENCE\RS\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3CA5D310-B7AD-44E9-9BBA-A83D2368BFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{14EF6A87-9ED0-4114-A1EE-4B1221F7E0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10905" yWindow="3270" windowWidth="24765" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,30 +45,23 @@
     <t>gemeente</t>
   </si>
   <si>
-    <t>BU15810004</t>
+    <t>Unknown</t>
   </si>
   <si>
-    <t>unknown</t>
+    <t>BU02220303</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="7"/>
-      <color rgb="FF212121"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,9 +84,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,12 +403,15 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,12 +419,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TERRA VERSION, REMOVED RASTER, RGDAL
</commit_message>
<xml_diff>
--- a/R/neighbourhoods.xlsx
+++ b/R/neighbourhoods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATASCIENCE\RS\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{14EF6A87-9ED0-4114-A1EE-4B1221F7E0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{66C024D1-5B5D-4E51-9FFC-F42F51731929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10905" yWindow="3270" windowWidth="24765" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3390" yWindow="630" windowWidth="24765" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <t>Unknown</t>
   </si>
   <si>
-    <t>BU02220303</t>
+    <t>BU15810004</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>